<commit_message>
Unittests fuer 'update_adresse' erstellt.
</commit_message>
<xml_diff>
--- a/src/main/update personenbezogene Daten/1 Update Adresse.xlsx
+++ b/src/main/update personenbezogene Daten/1 Update Adresse.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\update personenbezogene Daten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\test\testdaten_update_adresse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783CAEFA-312D-4F56-9600-1138A57AEDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A8AF55-70B5-4D36-854D-22D452603F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Daten</t>
   </si>
@@ -76,6 +77,21 @@
   </si>
   <si>
     <t>M100002</t>
+  </si>
+  <si>
+    <t>Ost_West_Ausland</t>
+  </si>
+  <si>
+    <t>Ort</t>
+  </si>
+  <si>
+    <t>Ost</t>
+  </si>
+  <si>
+    <t>West</t>
+  </si>
+  <si>
+    <t>Ausland</t>
   </si>
 </sst>
 </file>
@@ -119,11 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -404,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,71 +440,126 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA74EBE4-8FB2-4C0D-92C3-E4352DCE8DB8}">
+          <x14:formula1>
+            <xm:f>Tabelle2!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A308D98D-F0FD-4880-A217-094B57D0F94B}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>